<commit_message>
Add other tests groups
Data, script and slides about non plugin and non cli tests.
Add graph for cli tests.
</commit_message>
<xml_diff>
--- a/data/tempest_deps.xlsx
+++ b/data/tempest_deps.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1823" yWindow="518" windowWidth="31403" windowHeight="19178" tabRatio="500" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="1823" yWindow="518" windowWidth="31403" windowHeight="19178" tabRatio="500" firstSheet="10" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="tempest" sheetId="9" r:id="rId1"/>
@@ -24,6 +24,8 @@
     <sheet name="lib_detailed_graph_full" sheetId="21" r:id="rId10"/>
     <sheet name="plugins_over_time" sheetId="22" r:id="rId11"/>
     <sheet name="plugins_over_time_graph" sheetId="23" r:id="rId12"/>
+    <sheet name="cli_over_time" sheetId="24" r:id="rId13"/>
+    <sheet name="cli_over_time_graph" sheetId="25" r:id="rId14"/>
   </sheets>
   <definedNames>
     <definedName name="repo_per_lib_imports" localSheetId="3">lib!$A$1:$G$9</definedName>
@@ -33,6 +35,10 @@
     <definedName name="tempest_plugins" localSheetId="10">plugins_over_time!$A$2:$C$30</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
+  <webPublishing allowPng="1" targetScreenSize="1024x768" codePage="1252"/>
+  <webPublishObjects count="1">
+    <webPublishObject id="20872" divId="tempest_deps_20872" destinationFile="Z:\git\github.com\andreafrittoli\tempest_stable_interfaces\data\tempest_deps.htm" autoRepublish="1"/>
+  </webPublishObjects>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -129,7 +135,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="267">
   <si>
     <t>blazar</t>
   </si>
@@ -888,6 +894,48 @@
   </si>
   <si>
     <t>Label</t>
+  </si>
+  <si>
+    <t>Repos running CLI tests</t>
+  </si>
+  <si>
+    <t>python-aodhclient</t>
+  </si>
+  <si>
+    <t>python-ceilometerclient</t>
+  </si>
+  <si>
+    <t>python-cinderclient</t>
+  </si>
+  <si>
+    <t>python-glanceclient</t>
+  </si>
+  <si>
+    <t>python-gnocchiclient</t>
+  </si>
+  <si>
+    <t>python-heatclient</t>
+  </si>
+  <si>
+    <t>python-ironicclient</t>
+  </si>
+  <si>
+    <t>python-manilaclient</t>
+  </si>
+  <si>
+    <t>python-mistralclient</t>
+  </si>
+  <si>
+    <t>python-muranoclient</t>
+  </si>
+  <si>
+    <t>python-neutronclient</t>
+  </si>
+  <si>
+    <t>python-novaclient</t>
+  </si>
+  <si>
+    <t>python-saharaclient</t>
   </si>
 </sst>
 </file>
@@ -976,7 +1024,10 @@
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="32">
+  <dxfs count="33">
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0"/>
     </dxf>
@@ -1121,6 +1172,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1250,11 +1302,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="132278720"/>
-        <c:axId val="516678008"/>
+        <c:axId val="302826728"/>
+        <c:axId val="302827120"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="132278720"/>
+        <c:axId val="302826728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1274,7 +1326,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="516678008"/>
+        <c:crossAx val="302827120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1282,7 +1334,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="516678008"/>
+        <c:axId val="302827120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1307,7 +1359,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="132278720"/>
+        <c:crossAx val="302826728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1354,6 +1406,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1557,8 +1610,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="316628304"/>
-        <c:axId val="316622816"/>
+        <c:axId val="302827904"/>
+        <c:axId val="302828688"/>
       </c:barChart>
       <c:barChart>
         <c:barDir val="col"/>
@@ -1754,11 +1807,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="316626736"/>
-        <c:axId val="316624384"/>
+        <c:axId val="302829472"/>
+        <c:axId val="302829080"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="316628304"/>
+        <c:axId val="302827904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1778,7 +1831,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="316622816"/>
+        <c:crossAx val="302828688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1786,7 +1839,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="316622816"/>
+        <c:axId val="302828688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1811,12 +1864,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="316628304"/>
+        <c:crossAx val="302827904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="316624384"/>
+        <c:axId val="302829080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1842,12 +1895,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="316626736"/>
+        <c:crossAx val="302829472"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="316626736"/>
+        <c:axId val="302829472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1857,7 +1910,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="316624384"/>
+        <c:crossAx val="302829080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2016,11 +2069,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="316621640"/>
-        <c:axId val="316620856"/>
+        <c:axId val="304619392"/>
+        <c:axId val="304620176"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="316621640"/>
+        <c:axId val="304619392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2040,7 +2093,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="316620856"/>
+        <c:crossAx val="304620176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2048,7 +2101,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="316620856"/>
+        <c:axId val="304620176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2075,7 +2128,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="316621640"/>
+        <c:crossAx val="304619392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2295,11 +2348,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="316622424"/>
-        <c:axId val="316623208"/>
+        <c:axId val="304620568"/>
+        <c:axId val="304618608"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="316622424"/>
+        <c:axId val="304620568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2319,7 +2372,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="316623208"/>
+        <c:crossAx val="304618608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2327,7 +2380,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="316623208"/>
+        <c:axId val="304618608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2352,7 +2405,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="316622424"/>
+        <c:crossAx val="304620568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2526,11 +2579,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="316625952"/>
-        <c:axId val="316626344"/>
+        <c:axId val="304619784"/>
+        <c:axId val="304615864"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="316625952"/>
+        <c:axId val="304619784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2550,7 +2603,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="316626344"/>
+        <c:crossAx val="304615864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2558,7 +2611,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="316626344"/>
+        <c:axId val="304615864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2585,7 +2638,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="316625952"/>
+        <c:crossAx val="304619784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2759,11 +2812,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="328644224"/>
-        <c:axId val="328640304"/>
+        <c:axId val="304617824"/>
+        <c:axId val="304622136"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="328644224"/>
+        <c:axId val="304617824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2783,7 +2836,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="328640304"/>
+        <c:crossAx val="304622136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2791,7 +2844,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="328640304"/>
+        <c:axId val="304622136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2818,7 +2871,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="328644224"/>
+        <c:crossAx val="304617824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2904,7 +2957,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D1692F65-C602-42C2-8CC1-5BE4BED1490B}" type="CELLRANGE">
+                    <a:fld id="{7E5E8C8B-903E-431B-A64F-CB8F37057D64}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2935,7 +2988,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{172010D8-5E24-4124-B96B-234428976E36}" type="CELLRANGE">
+                    <a:fld id="{2EB8B691-707F-4541-88AD-99C45A758A75}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2967,7 +3020,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{84674DA4-1934-4910-B8CE-8A0DEC9614F1}" type="CELLRANGE">
+                    <a:fld id="{9EB7A7DB-2D83-45E2-86E5-19EC29B1C5B2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2999,7 +3052,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{162073F8-6BDF-42DE-A8A3-39F4D7DD24C3}" type="CELLRANGE">
+                    <a:fld id="{EAA2EF93-0CF8-4A84-87F7-17BB77E69E5B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3031,7 +3084,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DE4A5972-F05B-4067-8BBA-B2C3E69EEB92}" type="CELLRANGE">
+                    <a:fld id="{14337F6F-7492-4FD1-998F-E44856835700}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3063,7 +3116,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3033BF66-DF60-4E46-9E4E-28A9C67A2F11}" type="CELLRANGE">
+                    <a:fld id="{A014C59C-70EC-437B-807A-F615653ECF62}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3095,7 +3148,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4BC13D3F-77C7-4154-BDDA-BD33F0E87B31}" type="CELLRANGE">
+                    <a:fld id="{277573DC-B4C2-43E5-ABF1-DE36C914CA54}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3127,7 +3180,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0A4D2DE2-CA9C-46FC-94AA-64D9F2A9735B}" type="CELLRANGE">
+                    <a:fld id="{6D751515-D505-45D4-8467-8BBF20DEF99A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3159,7 +3212,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A22172FA-F021-4DCB-93CD-985074E83752}" type="CELLRANGE">
+                    <a:fld id="{50DFD2A4-0505-4499-82BB-7E8346584CF6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3191,7 +3244,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B8462B89-C6EF-4695-9AFB-A9F7251C7864}" type="CELLRANGE">
+                    <a:fld id="{DB926313-05B0-4D67-B410-09EBF569F337}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3223,7 +3276,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{62995BEC-B4EB-42D4-9E92-A87D6EED943E}" type="CELLRANGE">
+                    <a:fld id="{9A6FD0E1-9E70-44E1-BE41-2634780EA35B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3255,7 +3308,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{ED44AD29-FBB3-4551-888B-93FB386877C1}" type="CELLRANGE">
+                    <a:fld id="{36A24CE9-772A-42B1-A8AA-DD8DA3934B1A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3287,7 +3340,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2455A47F-EC5C-440E-9139-4E27EED5D92C}" type="CELLRANGE">
+                    <a:fld id="{5EE1EF31-4F0A-4002-9042-4E398F1295C5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3319,7 +3372,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{273EB385-E1C9-444A-B842-C8E2272B7755}" type="CELLRANGE">
+                    <a:fld id="{A83EBEED-854E-4F5D-8538-C78B6BC44BDC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3351,7 +3404,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DF244FE6-1DD6-47B4-9986-0989D7F47589}" type="CELLRANGE">
+                    <a:fld id="{F398EA54-835B-455F-B289-A14BCE8F4DD3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3383,7 +3436,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2BB75744-A4E5-45E7-86B7-F9DDF7571FED}" type="CELLRANGE">
+                    <a:fld id="{0AF2BE6D-CF7A-4F3B-A956-3E04DBAC46D8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3415,7 +3468,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{04BD6133-FC86-4646-BC0E-CA9AB4A819FF}" type="CELLRANGE">
+                    <a:fld id="{CF4D53F2-E1A3-478B-B71C-A88AD3AFC40E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3447,7 +3500,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{63040596-AB0D-4040-AD0C-93A4B986745F}" type="CELLRANGE">
+                    <a:fld id="{668D99BB-70C4-438B-B1A3-84AB596F9670}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3479,7 +3532,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DEB9B105-69B1-4C9F-AD0E-6816EA00232B}" type="CELLRANGE">
+                    <a:fld id="{6443DD75-0887-4918-92D2-C37AAFC163BE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3511,7 +3564,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{27C502B4-7B8D-451D-BDB7-0DC3D09156F7}" type="CELLRANGE">
+                    <a:fld id="{6E70BE38-6AFE-42D8-B83C-AA005551B3BA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3543,7 +3596,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{95B4827C-D375-41EF-B34A-866D8B248E9C}" type="CELLRANGE">
+                    <a:fld id="{0A9BBA19-630D-4E56-97B7-DF785A50A112}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3575,7 +3628,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EB5E429A-A3AE-4EE5-8693-6476ED18E159}" type="CELLRANGE">
+                    <a:fld id="{0DFF752D-7F0B-4D87-A71B-FF801FD9B89A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3607,7 +3660,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4922B888-965B-4FA3-B063-D72D1C0D4B19}" type="CELLRANGE">
+                    <a:fld id="{628EC5BD-91FC-45B3-97C8-DF1E870E5474}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3639,7 +3692,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{05A35097-1D17-44D8-A499-899B25EC961D}" type="CELLRANGE">
+                    <a:fld id="{B2DDCC46-9524-4940-8CCB-57B997B4B4F2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3671,7 +3724,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BF3B0545-566C-4DA3-A95A-8A9335DB712C}" type="CELLRANGE">
+                    <a:fld id="{85D58691-2AC5-41DF-BECF-FB1ABDF7CC91}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3703,7 +3756,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EDB86149-065F-44D7-82EC-272F2A37400C}" type="CELLRANGE">
+                    <a:fld id="{125B2B14-9840-444B-A02F-F6F76A179AEC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3735,7 +3788,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E5BB5E77-876F-4A93-8444-B0F5335DB916}" type="CELLRANGE">
+                    <a:fld id="{08CC9EA7-E96A-4FD9-AD31-CBDF00DD7E01}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3767,7 +3820,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5CAF23E5-7689-4A58-BC0B-E4A7D566B2EB}" type="CELLRANGE">
+                    <a:fld id="{B0D1D94E-DD44-4B09-A807-9ED9D4F6E324}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3799,7 +3852,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7F3F7560-54FB-490D-BC37-C63B332314C3}" type="CELLRANGE">
+                    <a:fld id="{A5A68AD9-DD1C-423E-AA98-228CEE0065E0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4150,11 +4203,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="328640696"/>
-        <c:axId val="328641088"/>
+        <c:axId val="304578320"/>
+        <c:axId val="304576752"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="328640696"/>
+        <c:axId val="304578320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4164,14 +4217,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="328641088"/>
+        <c:crossAx val="304576752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="328641088"/>
+        <c:axId val="304576752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4182,7 +4235,764 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="328640696"/>
+        <c:crossAx val="304578320"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Number of CLI tests over time</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="3.8029550024888462E-2"/>
+          <c:y val="8.5071844265759547E-2"/>
+          <c:w val="0.87245748278490132"/>
+          <c:h val="0.79155173785095045"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>cli_over_time!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Repos running CLI tests</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="950004"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{8DBB8D78-036D-4FC2-AEA2-DDBF836707BE}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{5DD84AC6-BE9C-4F85-B2AC-9F688918405F}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{37CA2229-7671-49FA-AFCB-9311C22E6530}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{1FDB019A-3E63-4AA1-A9DE-2677998F817A}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{A7593C3F-F06D-4AAE-A3F5-9C070A25562C}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{BBC477C3-84C5-4F48-9294-4A09C7AF6762}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{A76DD7A5-E1E5-4A1E-A93A-6B418997A888}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{884BFD9A-5F45-471C-B14B-95B6F519AA76}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="8"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{3E3BE5C3-0AB6-4990-9288-64B038A6814F}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="9"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{10DEA08C-7487-4CCE-BCF7-862272573446}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{B26B56F2-C1F5-4AB9-8221-D9D98E4629A2}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="11"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{C9E20DE0-11D7-4E5A-B4F6-023EFED27919}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="12"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{523DDBC8-5079-4BC0-BF08-96F5BC26034E}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="13"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{CD92A741-4DB5-440C-9EA7-95567E232F8D}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <a:prstGeom prst="rect">
+                    <a:avLst/>
+                  </a:prstGeom>
+                </c15:spPr>
+                <c15:layout/>
+                <c15:showDataLabelsRange val="1"/>
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>cli_over_time!$A$2:$A$15</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>41955</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41960</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42072</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>42087</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42112</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42115</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>42128</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>42133</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>42158</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>42244</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>42270</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>42307</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>42472</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>42472</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>cli_over_time!$B$2:$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:datalabelsRange>
+                <c15:f>cli_over_time!$C$2:$C$15</c15:f>
+                <c15:dlblRangeCache>
+                  <c:ptCount val="14"/>
+                  <c:pt idx="0">
+                    <c:v>python-manilaclient</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>python-mistralclient</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>python-neutronclient</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>python-saharaclient</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>python-glanceclient</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>python-novaclient</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>python-cinderclient</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>python-muranoclient</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>python-heatclient</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>python-gnocchiclient</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>python-designateclient</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>python-ironicclient</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>python-aodhclient</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>python-ceilometerclient</c:v>
+                  </c:pt>
+                </c15:dlblRangeCache>
+              </c15:datalabelsRange>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="291537904"/>
+        <c:axId val="291538296"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="291537904"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="291538296"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="291538296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="291537904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4220,7 +5030,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="120" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
@@ -4271,6 +5081,17 @@
   <webPublishItems count="1">
     <webPublishItem id="7644" divId="tempest_deps_7644" sourceType="chart" destinationFile="Z:\git\github.com\andreafrittoli\tempest_stable_interfaces\data\tmp\tempest_deps.htm"/>
   </webPublishItems>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="120" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </chartsheet>
 </file>
 
@@ -4440,7 +5261,34 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8654612" cy="6281573"/>
+    <xdr:ext cx="8659813" cy="6286500"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8659813" cy="6286500"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -4484,72 +5332,87 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G19" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G19" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
   <autoFilter ref="A1:G19"/>
   <sortState ref="A2:E19">
     <sortCondition descending="1" ref="C1:C19"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" name="import" dataDxfId="29"/>
-    <tableColumn id="2" name="namespace" dataDxfId="28"/>
-    <tableColumn id="3" name="count" dataDxfId="27"/>
-    <tableColumn id="7" name="pad_count" dataDxfId="26"/>
-    <tableColumn id="6" name="pad_total" dataDxfId="25"/>
-    <tableColumn id="4" name="total_count" dataDxfId="24"/>
-    <tableColumn id="5" name="repos" dataDxfId="23"/>
+    <tableColumn id="1" name="import" dataDxfId="30"/>
+    <tableColumn id="2" name="namespace" dataDxfId="29"/>
+    <tableColumn id="3" name="count" dataDxfId="28"/>
+    <tableColumn id="7" name="pad_count" dataDxfId="27"/>
+    <tableColumn id="6" name="pad_total" dataDxfId="26"/>
+    <tableColumn id="4" name="total_count" dataDxfId="25"/>
+    <tableColumn id="5" name="repos" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:G9" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:G9" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
   <autoFilter ref="A1:G9"/>
   <sortState ref="A2:E9">
     <sortCondition descending="1" ref="C1:C9"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" name="import" dataDxfId="20"/>
-    <tableColumn id="2" name="namespace" dataDxfId="19"/>
-    <tableColumn id="3" name="count" dataDxfId="18"/>
-    <tableColumn id="7" name="pad count" dataDxfId="17"/>
-    <tableColumn id="6" name="pad total" dataDxfId="16"/>
-    <tableColumn id="4" name="total_count" dataDxfId="15"/>
-    <tableColumn id="5" name="repos" dataDxfId="14"/>
+    <tableColumn id="1" name="import" dataDxfId="21"/>
+    <tableColumn id="2" name="namespace" dataDxfId="20"/>
+    <tableColumn id="3" name="count" dataDxfId="19"/>
+    <tableColumn id="7" name="pad count" dataDxfId="18"/>
+    <tableColumn id="6" name="pad total" dataDxfId="17"/>
+    <tableColumn id="4" name="total_count" dataDxfId="16"/>
+    <tableColumn id="5" name="repos" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:E51" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:E51" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="A1:E51"/>
   <sortState ref="A2:E51">
     <sortCondition descending="1" ref="C1:C51"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" name="import" dataDxfId="11"/>
-    <tableColumn id="2" name="namespace" dataDxfId="10"/>
-    <tableColumn id="3" name="count" dataDxfId="9"/>
-    <tableColumn id="4" name="total_count" dataDxfId="8"/>
-    <tableColumn id="5" name="repos" dataDxfId="7"/>
+    <tableColumn id="1" name="import" dataDxfId="12"/>
+    <tableColumn id="2" name="namespace" dataDxfId="11"/>
+    <tableColumn id="3" name="count" dataDxfId="10"/>
+    <tableColumn id="4" name="total_count" dataDxfId="9"/>
+    <tableColumn id="5" name="repos" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:E22" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:E22" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="A1:E22"/>
   <sortState ref="A2:E22">
     <sortCondition descending="1" ref="C1:C22"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" name="import" dataDxfId="4"/>
-    <tableColumn id="2" name="namespace" dataDxfId="3"/>
-    <tableColumn id="3" name="count" dataDxfId="2"/>
-    <tableColumn id="4" name="total_count" dataDxfId="1"/>
-    <tableColumn id="5" name="repos" dataDxfId="0"/>
+    <tableColumn id="1" name="import" dataDxfId="5"/>
+    <tableColumn id="2" name="namespace" dataDxfId="4"/>
+    <tableColumn id="3" name="count" dataDxfId="3"/>
+    <tableColumn id="4" name="total_count" dataDxfId="2"/>
+    <tableColumn id="5" name="repos" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:C15" totalsRowShown="0">
+  <autoFilter ref="A1:C15"/>
+  <sortState ref="A2:C15">
+    <sortCondition ref="A1:A15"/>
+  </sortState>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Date" dataDxfId="0"/>
+    <tableColumn id="2" name="Repos running CLI tests"/>
+    <tableColumn id="3" name="Label"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6784,7 +7647,7 @@
   <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -7132,4 +7995,192 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="1" width="10.1875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.4375" customWidth="1"/>
+    <col min="3" max="3" width="20.5625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A2" s="3">
+        <v>41955</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A3" s="3">
+        <v>41960</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A4" s="3">
+        <v>42072</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A5" s="3">
+        <v>42087</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A6" s="3">
+        <v>42112</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A7" s="3">
+        <v>42115</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A8" s="3">
+        <v>42128</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A9" s="3">
+        <v>42133</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A10" s="3">
+        <v>42158</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A11" s="3">
+        <v>42244</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A12" s="3">
+        <v>42270</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A13" s="3">
+        <v>42307</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A14" s="3">
+        <v>42472</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A15" s="3">
+        <v>42472</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>255</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>